<commit_message>
Changed SampleName to not include downstream use of filter
</commit_message>
<xml_diff>
--- a/protocols/GEODES Datasheets.xlsx
+++ b/protocols/GEODES Datasheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\geodes\protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
   <si>
     <t>DATE:</t>
   </si>
@@ -283,15 +283,6 @@
     <t>Bacterial production assays should be started at MSB within 1/2 hour of collection.</t>
   </si>
   <si>
-    <t>GEODES_ME_0hr_RNA</t>
-  </si>
-  <si>
-    <t>GEODES_ME_0hr_DNA</t>
-  </si>
-  <si>
-    <t>GEODES_ME_0hr_SAG</t>
-  </si>
-  <si>
     <t>GEODES001</t>
   </si>
   <si>
@@ -326,6 +317,9 @@
   </si>
   <si>
     <t>PAR start time:</t>
+  </si>
+  <si>
+    <t>GEODES_ME_0hr</t>
   </si>
 </sst>
 </file>
@@ -804,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -826,7 +820,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -959,7 +953,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +967,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,10 +1017,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1037,10 +1031,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1051,10 +1045,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1065,10 +1059,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1079,10 +1073,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1093,10 +1087,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>27</v>
@@ -1111,10 +1105,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>27</v>
@@ -1245,7 +1239,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -1534,7 +1528,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H26" s="6"/>
     </row>

</xml_diff>

<commit_message>
Updated ordering sheet and metadata sheets based on input by Robin and Josh
</commit_message>
<xml_diff>
--- a/protocols/GEODES Datasheets.xlsx
+++ b/protocols/GEODES Datasheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\geodes\protocols\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\geodes\protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
   <si>
     <t>DATE:</t>
   </si>
@@ -190,9 +190,6 @@
     <t>SECCHI DEPTH:</t>
   </si>
   <si>
-    <t>Enter time collected:</t>
-  </si>
-  <si>
     <t>LAKE:</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>Charge sonde battery if needed</t>
   </si>
   <si>
-    <t>Time filtered</t>
-  </si>
-  <si>
     <t>Phytoplankton bottle</t>
   </si>
   <si>
@@ -320,6 +314,15 @@
   </si>
   <si>
     <t>GEODES_ME_0hr</t>
+  </si>
+  <si>
+    <t>Time finished</t>
+  </si>
+  <si>
+    <t>Enter time collected for each replicate sample:</t>
+  </si>
+  <si>
+    <t>Sample Depth</t>
   </si>
 </sst>
 </file>
@@ -712,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -723,7 +726,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -798,7 +801,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -820,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -886,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -928,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -937,7 +940,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,7 +948,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -953,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -964,10 +967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,15 +978,16 @@
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -995,7 +999,7 @@
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1003,130 +1007,154 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>27</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>27</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1134,18 +1162,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1217,7 +1245,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -1239,10 +1267,10 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1251,10 +1279,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -1528,7 +1556,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H26" s="6"/>
     </row>
@@ -1686,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1698,7 +1726,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -1733,7 +1761,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,7 +1785,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1781,7 +1809,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,7 +1817,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,46 +1825,46 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1850,7 +1878,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1890,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -1896,7 +1924,7 @@
         <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1972,10 +2000,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2001,7 +2029,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>